<commit_message>
Pages Panel GUI Main & Test
</commit_message>
<xml_diff>
--- a/Wordpress_manual_Testcases All 6 modules - 30TC.xlsx
+++ b/Wordpress_manual_Testcases All 6 modules - 30TC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kushal_ghosh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://persistentsystems-my.sharepoint.com/personal/kushal_ghosh_persistent_com/Documents/Documents/MPWP/Miniproject_Team6/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5876B7A-4926-4A65-A82F-0633274BB476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -885,24 +885,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2025,8 +2025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F8FCF9A-FA5B-48C7-8502-E9C4A72ACD8D}">
   <dimension ref="A1:L241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B215" sqref="B215:B237"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="E237" sqref="E237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2091,13 +2091,13 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="24" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -2109,21 +2109,21 @@
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="24" t="s">
         <v>9</v>
       </c>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="23"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
@@ -2136,14 +2136,14 @@
       <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="20"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="23"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
@@ -2153,13 +2153,13 @@
       <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="23"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
       <c r="E6" s="1" t="s">
         <v>32</v>
       </c>
@@ -2172,13 +2172,13 @@
       <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="1" t="s">
         <v>49</v>
       </c>
@@ -2188,31 +2188,31 @@
       <c r="G7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
       <c r="E8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
     </row>
     <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23"/>
+      <c r="B9" s="22"/>
     </row>
     <row r="10" spans="1:12" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="24" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -2224,23 +2224,23 @@
       <c r="G10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="20" t="s">
+      <c r="K10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="L10" s="23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="23"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2253,15 +2253,15 @@
       <c r="H11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="21"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="23"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="23"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="1" t="s">
         <v>30</v>
       </c>
@@ -2271,14 +2271,14 @@
       <c r="G12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="L12" s="21"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="L12" s="23"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="23"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="1" t="s">
         <v>32</v>
       </c>
@@ -2291,14 +2291,14 @@
       <c r="H13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="L13" s="21"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="L13" s="23"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="23"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="1" t="s">
         <v>49</v>
       </c>
@@ -2308,33 +2308,33 @@
       <c r="G14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="L14" s="21"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="L14" s="23"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="23"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="L15" s="21"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="L15" s="23"/>
     </row>
     <row r="16" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="23"/>
+      <c r="B16" s="22"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="20" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="24" t="s">
         <v>37</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -2346,23 +2346,23 @@
       <c r="G17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="K17" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L17" s="21" t="s">
+      <c r="L17" s="23" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="23"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="1" t="s">
         <v>10</v>
       </c>
@@ -2375,15 +2375,15 @@
       <c r="H18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="21"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="23"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="23"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="1" t="s">
         <v>30</v>
       </c>
@@ -2393,14 +2393,14 @@
       <c r="G19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="L19" s="21"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="L19" s="23"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="23"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="1" t="s">
         <v>32</v>
       </c>
@@ -2413,14 +2413,14 @@
       <c r="H20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="L20" s="21"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="L20" s="23"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="23"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="1" t="s">
         <v>49</v>
       </c>
@@ -2430,33 +2430,33 @@
       <c r="G21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="L21" s="21"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="L21" s="23"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="23"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
       <c r="E22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="L22" s="21"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="L22" s="23"/>
     </row>
     <row r="23" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="23"/>
+      <c r="B23" s="22"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="20" t="s">
+      <c r="B24" s="22"/>
+      <c r="C24" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="24" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -2468,23 +2468,23 @@
       <c r="G24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="20" t="s">
+      <c r="I24" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="20" t="s">
+      <c r="J24" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="K24" s="20" t="s">
+      <c r="K24" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L24" s="21" t="s">
+      <c r="L24" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="23"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
       <c r="E25" s="1" t="s">
         <v>10</v>
       </c>
@@ -2497,15 +2497,15 @@
       <c r="H25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="21"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="23"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="23"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
       <c r="E26" s="1" t="s">
         <v>30</v>
       </c>
@@ -2515,14 +2515,14 @@
       <c r="G26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="L26" s="21"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="L26" s="23"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="23"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
       <c r="E27" s="1" t="s">
         <v>32</v>
       </c>
@@ -2535,14 +2535,14 @@
       <c r="H27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="L27" s="21"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="L27" s="23"/>
     </row>
     <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="23"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
       <c r="E28" s="1" t="s">
         <v>49</v>
       </c>
@@ -2552,33 +2552,33 @@
       <c r="G28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="L28" s="21"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="L28" s="23"/>
     </row>
     <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="23"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
       <c r="E29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="L29" s="21"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="L29" s="23"/>
     </row>
     <row r="30" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="23"/>
+      <c r="B30" s="22"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="20" t="s">
+      <c r="B31" s="22"/>
+      <c r="C31" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="24" t="s">
         <v>51</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -2590,10 +2590,10 @@
       <c r="G31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I31" s="21" t="s">
+      <c r="I31" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="J31" s="21" t="s">
+      <c r="J31" s="23" t="s">
         <v>50</v>
       </c>
       <c r="K31" s="1" t="s">
@@ -2601,9 +2601,9 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="23"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
       <c r="E32" s="1" t="s">
         <v>10</v>
       </c>
@@ -2616,13 +2616,13 @@
       <c r="H32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B33" s="23"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
       <c r="E33" s="1" t="s">
         <v>30</v>
       </c>
@@ -2632,13 +2632,13 @@
       <c r="G33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B34" s="23"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
       <c r="E34" s="1" t="s">
         <v>32</v>
       </c>
@@ -2651,13 +2651,13 @@
       <c r="H34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B35" s="23"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
       <c r="E35" s="1" t="s">
         <v>49</v>
       </c>
@@ -2667,13 +2667,13 @@
       <c r="G35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B36" s="23"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
       <c r="E36" s="1" t="s">
         <v>38</v>
       </c>
@@ -2683,34 +2683,34 @@
       <c r="G36" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B37" s="23"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
       <c r="F37" s="1">
         <v>6</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
     </row>
     <row r="38" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="23"/>
+      <c r="B38" s="22"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="20" t="s">
+      <c r="B39" s="22"/>
+      <c r="C39" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="24" t="s">
         <v>52</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -2722,23 +2722,23 @@
       <c r="G39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I39" s="21" t="s">
+      <c r="I39" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="J39" s="21" t="s">
+      <c r="J39" s="23" t="s">
         <v>56</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L39" s="22" t="s">
+      <c r="L39" s="26" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B40" s="23"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
       <c r="E40" s="1" t="s">
         <v>10</v>
       </c>
@@ -2748,14 +2748,14 @@
       <c r="G40" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="L40" s="22"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="L40" s="26"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B41" s="23"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
       <c r="E41" s="1" t="s">
         <v>30</v>
       </c>
@@ -2768,14 +2768,14 @@
       <c r="H41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="L41" s="22"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="L41" s="26"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B42" s="23"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
       <c r="E42" s="1" t="s">
         <v>32</v>
       </c>
@@ -2785,36 +2785,36 @@
       <c r="G42" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="L42" s="22"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
+      <c r="L42" s="26"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B43" s="23"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
       <c r="E43" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="L43" s="22"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="L43" s="26"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B44" s="23"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
       <c r="E44" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
-      <c r="L44" s="22"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
+      <c r="L44" s="26"/>
     </row>
     <row r="45" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B45" s="5"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
       <c r="L45" s="4"/>
     </row>
     <row r="46" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -2827,13 +2827,13 @@
       <c r="A49" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B49" s="23" t="s">
+      <c r="B49" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="C49" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="D49" s="21" t="s">
+      <c r="D49" s="23" t="s">
         <v>136</v>
       </c>
       <c r="E49" s="1" t="s">
@@ -2845,23 +2845,23 @@
       <c r="G49" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I49" s="21" t="s">
+      <c r="I49" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="J49" s="21" t="s">
+      <c r="J49" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="K49" s="20" t="s">
+      <c r="K49" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L49" s="21" t="s">
+      <c r="L49" s="23" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="23"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
       <c r="E50" s="1" t="s">
         <v>10</v>
       </c>
@@ -2871,15 +2871,15 @@
       <c r="G50" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="21"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="23"/>
+      <c r="K50" s="24"/>
+      <c r="L50" s="23"/>
     </row>
     <row r="51" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="23"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
       <c r="E51" s="1" t="s">
         <v>30</v>
       </c>
@@ -2889,14 +2889,14 @@
       <c r="G51" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I51" s="21"/>
-      <c r="J51" s="21"/>
-      <c r="L51" s="21"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
+      <c r="L51" s="23"/>
     </row>
     <row r="52" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="23"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
       <c r="E52" s="1" t="s">
         <v>32</v>
       </c>
@@ -2906,14 +2906,14 @@
       <c r="G52" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I52" s="21"/>
-      <c r="J52" s="21"/>
-      <c r="L52" s="21"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="23"/>
+      <c r="L52" s="23"/>
     </row>
     <row r="53" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="23"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
       <c r="E53" s="1" t="s">
         <v>69</v>
       </c>
@@ -2923,14 +2923,14 @@
       <c r="G53" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I53" s="21"/>
-      <c r="J53" s="21"/>
-      <c r="L53" s="21"/>
+      <c r="I53" s="23"/>
+      <c r="J53" s="23"/>
+      <c r="L53" s="23"/>
     </row>
     <row r="54" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="23"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
       <c r="E54" s="1" t="s">
         <v>38</v>
       </c>
@@ -2940,12 +2940,12 @@
       <c r="G54" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I54" s="21"/>
-      <c r="J54" s="21"/>
-      <c r="L54" s="21"/>
+      <c r="I54" s="23"/>
+      <c r="J54" s="23"/>
+      <c r="L54" s="23"/>
     </row>
     <row r="55" spans="1:12" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="23"/>
+      <c r="B55" s="22"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
     </row>
@@ -2953,11 +2953,11 @@
       <c r="A56" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="21" t="s">
+      <c r="B56" s="22"/>
+      <c r="C56" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="D56" s="21" t="s">
+      <c r="D56" s="23" t="s">
         <v>216</v>
       </c>
       <c r="E56" s="19" t="s">
@@ -2969,10 +2969,10 @@
       <c r="G56" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="I56" s="26" t="s">
+      <c r="I56" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="J56" s="26" t="s">
+      <c r="J56" s="25" t="s">
         <v>220</v>
       </c>
       <c r="K56" s="14" t="s">
@@ -2980,9 +2980,9 @@
       </c>
     </row>
     <row r="57" spans="1:12" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="23"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
+      <c r="B57" s="22"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
       <c r="E57" s="19" t="s">
         <v>10</v>
       </c>
@@ -2992,13 +2992,13 @@
       <c r="G57" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="I57" s="26"/>
-      <c r="J57" s="26"/>
+      <c r="I57" s="25"/>
+      <c r="J57" s="25"/>
     </row>
     <row r="58" spans="1:12" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="23"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
       <c r="E58" s="19" t="s">
         <v>30</v>
       </c>
@@ -3008,13 +3008,13 @@
       <c r="G58" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="I58" s="26"/>
-      <c r="J58" s="26"/>
+      <c r="I58" s="25"/>
+      <c r="J58" s="25"/>
     </row>
     <row r="59" spans="1:12" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="23"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
       <c r="E59" s="19" t="s">
         <v>32</v>
       </c>
@@ -3027,13 +3027,13 @@
       <c r="H59" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="I59" s="26"/>
-      <c r="J59" s="26"/>
+      <c r="I59" s="25"/>
+      <c r="J59" s="25"/>
     </row>
     <row r="60" spans="1:12" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="23"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
       <c r="E60" s="19" t="s">
         <v>69</v>
       </c>
@@ -3043,13 +3043,13 @@
       <c r="G60" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="I60" s="26"/>
-      <c r="J60" s="26"/>
+      <c r="I60" s="25"/>
+      <c r="J60" s="25"/>
     </row>
     <row r="61" spans="1:12" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="23"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
       <c r="E61" s="19" t="s">
         <v>38</v>
       </c>
@@ -3059,11 +3059,11 @@
       <c r="G61" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="I61" s="26"/>
-      <c r="J61" s="26"/>
+      <c r="I61" s="25"/>
+      <c r="J61" s="25"/>
     </row>
     <row r="62" spans="1:12" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="23"/>
+      <c r="B62" s="22"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
     </row>
@@ -3071,11 +3071,11 @@
       <c r="A63" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="21" t="s">
+      <c r="B63" s="22"/>
+      <c r="C63" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="D63" s="21" t="s">
+      <c r="D63" s="23" t="s">
         <v>75</v>
       </c>
       <c r="E63" s="1" t="s">
@@ -3087,20 +3087,20 @@
       <c r="G63" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I63" s="21" t="s">
+      <c r="I63" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="J63" s="21" t="s">
+      <c r="J63" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="K63" s="20" t="s">
+      <c r="K63" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="23"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
       <c r="E64" s="1" t="s">
         <v>10</v>
       </c>
@@ -3113,14 +3113,14 @@
       <c r="H64" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I64" s="21"/>
-      <c r="J64" s="21"/>
-      <c r="K64" s="20"/>
+      <c r="I64" s="23"/>
+      <c r="J64" s="23"/>
+      <c r="K64" s="24"/>
     </row>
     <row r="65" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="23"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
+      <c r="B65" s="22"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
       <c r="E65" s="1" t="s">
         <v>30</v>
       </c>
@@ -3130,51 +3130,51 @@
       <c r="G65" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I65" s="21"/>
-      <c r="J65" s="21"/>
+      <c r="I65" s="23"/>
+      <c r="J65" s="23"/>
     </row>
     <row r="66" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="23"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
+      <c r="B66" s="22"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
       <c r="E66" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I66" s="21"/>
-      <c r="J66" s="21"/>
+      <c r="I66" s="23"/>
+      <c r="J66" s="23"/>
     </row>
     <row r="67" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="23"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
+      <c r="B67" s="22"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
       <c r="E67" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I67" s="21"/>
-      <c r="J67" s="21"/>
+      <c r="I67" s="23"/>
+      <c r="J67" s="23"/>
     </row>
     <row r="68" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="23"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
       <c r="E68" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I68" s="21"/>
-      <c r="J68" s="21"/>
+      <c r="I68" s="23"/>
+      <c r="J68" s="23"/>
     </row>
     <row r="69" spans="1:12" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="23"/>
+      <c r="B69" s="22"/>
     </row>
     <row r="70" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="23"/>
-      <c r="C70" s="21" t="s">
+      <c r="B70" s="22"/>
+      <c r="C70" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="D70" s="21" t="s">
+      <c r="D70" s="23" t="s">
         <v>76</v>
       </c>
       <c r="E70" s="10" t="s">
@@ -3189,23 +3189,23 @@
       <c r="H70" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I70" s="20" t="s">
+      <c r="I70" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="J70" s="20" t="s">
+      <c r="J70" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="K70" s="20" t="s">
+      <c r="K70" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L70" s="20" t="s">
+      <c r="L70" s="24" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="23"/>
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
       <c r="E71" s="10" t="s">
         <v>10</v>
       </c>
@@ -3215,15 +3215,15 @@
       <c r="G71" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I71" s="20"/>
-      <c r="J71" s="20"/>
-      <c r="K71" s="20"/>
-      <c r="L71" s="20"/>
+      <c r="I71" s="24"/>
+      <c r="J71" s="24"/>
+      <c r="K71" s="24"/>
+      <c r="L71" s="24"/>
     </row>
     <row r="72" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="23"/>
-      <c r="C72" s="21"/>
-      <c r="D72" s="21"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
       <c r="E72" s="10" t="s">
         <v>30</v>
       </c>
@@ -3233,42 +3233,42 @@
       <c r="G72" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I72" s="20"/>
-      <c r="J72" s="20"/>
-      <c r="L72" s="20"/>
+      <c r="I72" s="24"/>
+      <c r="J72" s="24"/>
+      <c r="L72" s="24"/>
     </row>
     <row r="73" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="23"/>
-      <c r="C73" s="21"/>
-      <c r="D73" s="21"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
       <c r="E73" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I73" s="20"/>
-      <c r="J73" s="20"/>
-      <c r="L73" s="20"/>
+      <c r="I73" s="24"/>
+      <c r="J73" s="24"/>
+      <c r="L73" s="24"/>
     </row>
     <row r="74" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="23"/>
-      <c r="C74" s="21"/>
-      <c r="D74" s="21"/>
+      <c r="B74" s="22"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
       <c r="E74" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="I74" s="20"/>
-      <c r="J74" s="20"/>
-      <c r="L74" s="20"/>
+      <c r="I74" s="24"/>
+      <c r="J74" s="24"/>
+      <c r="L74" s="24"/>
     </row>
     <row r="75" spans="1:12" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="23"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
       <c r="E75" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I75" s="20"/>
-      <c r="J75" s="20"/>
-      <c r="L75" s="20"/>
+      <c r="I75" s="24"/>
+      <c r="J75" s="24"/>
+      <c r="L75" s="24"/>
     </row>
     <row r="76" spans="1:12" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="13"/>
@@ -3277,13 +3277,13 @@
       <c r="A77" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B77" s="23" t="s">
+      <c r="B77" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="C77" s="21" t="s">
+      <c r="C77" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="D77" s="21" t="s">
+      <c r="D77" s="23" t="s">
         <v>169</v>
       </c>
       <c r="E77" s="10" t="s">
@@ -3298,23 +3298,23 @@
       <c r="H77" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="I77" s="21" t="s">
+      <c r="I77" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="J77" s="21" t="s">
+      <c r="J77" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="K77" s="20" t="s">
+      <c r="K77" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L77" s="21" t="s">
+      <c r="L77" s="23" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:12" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="23"/>
-      <c r="C78" s="21"/>
-      <c r="D78" s="21"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="23"/>
+      <c r="D78" s="23"/>
       <c r="E78" s="10" t="s">
         <v>10</v>
       </c>
@@ -3327,15 +3327,15 @@
       <c r="H78" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="I78" s="21"/>
-      <c r="J78" s="21"/>
-      <c r="K78" s="20"/>
-      <c r="L78" s="21"/>
+      <c r="I78" s="23"/>
+      <c r="J78" s="23"/>
+      <c r="K78" s="24"/>
+      <c r="L78" s="23"/>
     </row>
     <row r="79" spans="1:12" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="23"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="23"/>
       <c r="E79" s="10" t="s">
         <v>30</v>
       </c>
@@ -3345,14 +3345,14 @@
       <c r="G79" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="I79" s="21"/>
-      <c r="J79" s="21"/>
-      <c r="L79" s="21"/>
+      <c r="I79" s="23"/>
+      <c r="J79" s="23"/>
+      <c r="L79" s="23"/>
     </row>
     <row r="80" spans="1:12" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="23"/>
-      <c r="C80" s="21"/>
-      <c r="D80" s="21"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
       <c r="E80" s="10" t="s">
         <v>32</v>
       </c>
@@ -3365,14 +3365,14 @@
       <c r="H80" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="I80" s="21"/>
-      <c r="J80" s="21"/>
-      <c r="L80" s="21"/>
+      <c r="I80" s="23"/>
+      <c r="J80" s="23"/>
+      <c r="L80" s="23"/>
     </row>
     <row r="81" spans="1:12" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="23"/>
-      <c r="C81" s="21"/>
-      <c r="D81" s="21"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
       <c r="E81" s="10" t="s">
         <v>170</v>
       </c>
@@ -3382,14 +3382,14 @@
       <c r="G81" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="I81" s="21"/>
-      <c r="J81" s="21"/>
-      <c r="L81" s="21"/>
+      <c r="I81" s="23"/>
+      <c r="J81" s="23"/>
+      <c r="L81" s="23"/>
     </row>
     <row r="82" spans="1:12" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="23"/>
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
       <c r="E82" s="10" t="s">
         <v>38</v>
       </c>
@@ -3402,12 +3402,12 @@
       <c r="H82" s="10">
         <v>3</v>
       </c>
-      <c r="I82" s="21"/>
-      <c r="J82" s="21"/>
-      <c r="L82" s="21"/>
+      <c r="I82" s="23"/>
+      <c r="J82" s="23"/>
+      <c r="L82" s="23"/>
     </row>
     <row r="83" spans="1:12" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="23"/>
+      <c r="B83" s="22"/>
       <c r="C83" s="9"/>
       <c r="D83" s="9"/>
     </row>
@@ -3415,11 +3415,11 @@
       <c r="A84" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="B84" s="23"/>
-      <c r="C84" s="26" t="s">
+      <c r="B84" s="22"/>
+      <c r="C84" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="D84" s="26" t="s">
+      <c r="D84" s="25" t="s">
         <v>219</v>
       </c>
       <c r="E84" s="19" t="s">
@@ -3436,9 +3436,9 @@
       </c>
     </row>
     <row r="85" spans="1:12" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="23"/>
-      <c r="C85" s="26"/>
-      <c r="D85" s="26"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="25"/>
+      <c r="D85" s="25"/>
       <c r="E85" s="19" t="s">
         <v>10</v>
       </c>
@@ -3453,9 +3453,9 @@
       </c>
     </row>
     <row r="86" spans="1:12" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="23"/>
-      <c r="C86" s="26"/>
-      <c r="D86" s="26"/>
+      <c r="B86" s="22"/>
+      <c r="C86" s="25"/>
+      <c r="D86" s="25"/>
       <c r="E86" s="19" t="s">
         <v>30</v>
       </c>
@@ -3468,9 +3468,9 @@
       <c r="H86" s="19"/>
     </row>
     <row r="87" spans="1:12" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="23"/>
-      <c r="C87" s="26"/>
-      <c r="D87" s="26"/>
+      <c r="B87" s="22"/>
+      <c r="C87" s="25"/>
+      <c r="D87" s="25"/>
       <c r="E87" s="19" t="s">
         <v>32</v>
       </c>
@@ -3485,9 +3485,9 @@
       </c>
     </row>
     <row r="88" spans="1:12" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="23"/>
-      <c r="C88" s="26"/>
-      <c r="D88" s="26"/>
+      <c r="B88" s="22"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="25"/>
       <c r="E88" s="19" t="s">
         <v>170</v>
       </c>
@@ -3500,9 +3500,9 @@
       <c r="H88" s="19"/>
     </row>
     <row r="89" spans="1:12" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="23"/>
-      <c r="C89" s="26"/>
-      <c r="D89" s="26"/>
+      <c r="B89" s="22"/>
+      <c r="C89" s="25"/>
+      <c r="D89" s="25"/>
       <c r="E89" s="19" t="s">
         <v>38</v>
       </c>
@@ -3517,9 +3517,9 @@
       </c>
     </row>
     <row r="90" spans="1:12" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="23"/>
-      <c r="C90" s="26"/>
-      <c r="D90" s="26"/>
+      <c r="B90" s="22"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="25"/>
       <c r="F90" s="19">
         <v>7</v>
       </c>
@@ -3531,9 +3531,9 @@
       </c>
     </row>
     <row r="91" spans="1:12" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="23"/>
-      <c r="C91" s="26"/>
-      <c r="D91" s="26"/>
+      <c r="B91" s="22"/>
+      <c r="C91" s="25"/>
+      <c r="D91" s="25"/>
       <c r="F91" s="19">
         <v>8</v>
       </c>
@@ -3543,44 +3543,44 @@
       <c r="H91" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="I91" s="24"/>
-      <c r="J91" s="24"/>
+      <c r="I91" s="20"/>
+      <c r="J91" s="20"/>
       <c r="K91" s="3"/>
     </row>
     <row r="92" spans="1:12" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="23"/>
-      <c r="C92" s="26"/>
-      <c r="D92" s="26"/>
+      <c r="B92" s="22"/>
+      <c r="C92" s="25"/>
+      <c r="D92" s="25"/>
       <c r="F92" s="19">
         <v>9</v>
       </c>
       <c r="G92" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="I92" s="24"/>
-      <c r="J92" s="24"/>
+      <c r="I92" s="20"/>
+      <c r="J92" s="20"/>
       <c r="K92" s="3"/>
     </row>
     <row r="93" spans="1:12" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="23"/>
-      <c r="C93" s="26"/>
-      <c r="D93" s="26"/>
+      <c r="B93" s="22"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="25"/>
       <c r="F93" s="19">
         <v>10</v>
       </c>
       <c r="G93" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="I93" s="24"/>
-      <c r="J93" s="24"/>
+      <c r="I93" s="20"/>
+      <c r="J93" s="20"/>
       <c r="K93" s="19"/>
     </row>
     <row r="94" spans="1:12" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="25"/>
-      <c r="C94" s="24"/>
-      <c r="D94" s="24"/>
-      <c r="I94" s="24"/>
-      <c r="J94" s="24"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="20"/>
+      <c r="D94" s="20"/>
+      <c r="I94" s="20"/>
+      <c r="J94" s="20"/>
       <c r="K94" s="19"/>
     </row>
     <row r="95" spans="1:12" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3596,13 +3596,13 @@
       <c r="A98" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B98" s="23" t="s">
+      <c r="B98" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="C98" s="20" t="s">
+      <c r="C98" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D98" s="20" t="s">
+      <c r="D98" s="24" t="s">
         <v>92</v>
       </c>
       <c r="E98" s="1" t="s">
@@ -3617,23 +3617,23 @@
       <c r="H98" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="I98" s="21" t="s">
+      <c r="I98" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="J98" s="21" t="s">
+      <c r="J98" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="K98" s="20" t="s">
+      <c r="K98" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L98" s="21" t="s">
+      <c r="L98" s="23" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B99" s="23"/>
-      <c r="C99" s="20"/>
-      <c r="D99" s="20"/>
+      <c r="B99" s="22"/>
+      <c r="C99" s="24"/>
+      <c r="D99" s="24"/>
       <c r="E99" s="1" t="s">
         <v>10</v>
       </c>
@@ -3643,15 +3643,15 @@
       <c r="G99" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I99" s="21"/>
-      <c r="J99" s="21"/>
-      <c r="K99" s="20"/>
-      <c r="L99" s="21"/>
+      <c r="I99" s="23"/>
+      <c r="J99" s="23"/>
+      <c r="K99" s="24"/>
+      <c r="L99" s="23"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B100" s="23"/>
-      <c r="C100" s="20"/>
-      <c r="D100" s="20"/>
+      <c r="B100" s="22"/>
+      <c r="C100" s="24"/>
+      <c r="D100" s="24"/>
       <c r="E100" s="1" t="s">
         <v>30</v>
       </c>
@@ -3661,14 +3661,14 @@
       <c r="G100" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I100" s="21"/>
-      <c r="J100" s="21"/>
-      <c r="L100" s="21"/>
+      <c r="I100" s="23"/>
+      <c r="J100" s="23"/>
+      <c r="L100" s="23"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B101" s="23"/>
-      <c r="C101" s="20"/>
-      <c r="D101" s="20"/>
+      <c r="B101" s="22"/>
+      <c r="C101" s="24"/>
+      <c r="D101" s="24"/>
       <c r="E101" s="1" t="s">
         <v>32</v>
       </c>
@@ -3678,14 +3678,14 @@
       <c r="G101" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I101" s="21"/>
-      <c r="J101" s="21"/>
-      <c r="L101" s="21"/>
+      <c r="I101" s="23"/>
+      <c r="J101" s="23"/>
+      <c r="L101" s="23"/>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B102" s="23"/>
-      <c r="C102" s="20"/>
-      <c r="D102" s="20"/>
+      <c r="B102" s="22"/>
+      <c r="C102" s="24"/>
+      <c r="D102" s="24"/>
       <c r="E102" s="1" t="s">
         <v>91</v>
       </c>
@@ -3695,33 +3695,33 @@
       <c r="G102" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I102" s="21"/>
-      <c r="J102" s="21"/>
-      <c r="L102" s="21"/>
+      <c r="I102" s="23"/>
+      <c r="J102" s="23"/>
+      <c r="L102" s="23"/>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B103" s="23"/>
-      <c r="C103" s="20"/>
-      <c r="D103" s="20"/>
+      <c r="B103" s="22"/>
+      <c r="C103" s="24"/>
+      <c r="D103" s="24"/>
       <c r="E103" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I103" s="21"/>
-      <c r="J103" s="21"/>
-      <c r="L103" s="21"/>
+      <c r="I103" s="23"/>
+      <c r="J103" s="23"/>
+      <c r="L103" s="23"/>
     </row>
     <row r="104" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="23"/>
+      <c r="B104" s="22"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B105" s="23"/>
-      <c r="C105" s="20" t="s">
+      <c r="B105" s="22"/>
+      <c r="C105" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="D105" s="20" t="s">
+      <c r="D105" s="24" t="s">
         <v>106</v>
       </c>
       <c r="E105" s="1" t="s">
@@ -3733,23 +3733,23 @@
       <c r="G105" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="I105" s="21" t="s">
+      <c r="I105" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="J105" s="21" t="s">
+      <c r="J105" s="23" t="s">
         <v>112</v>
       </c>
       <c r="K105" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L105" s="20" t="s">
+      <c r="L105" s="24" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="23"/>
-      <c r="C106" s="20"/>
-      <c r="D106" s="20"/>
+      <c r="B106" s="22"/>
+      <c r="C106" s="24"/>
+      <c r="D106" s="24"/>
       <c r="E106" s="1" t="s">
         <v>10</v>
       </c>
@@ -3762,77 +3762,77 @@
       <c r="H106" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="I106" s="21"/>
-      <c r="J106" s="21"/>
-      <c r="L106" s="20"/>
+      <c r="I106" s="23"/>
+      <c r="J106" s="23"/>
+      <c r="L106" s="24"/>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B107" s="23"/>
-      <c r="C107" s="20"/>
-      <c r="D107" s="20"/>
+      <c r="B107" s="22"/>
+      <c r="C107" s="24"/>
+      <c r="D107" s="24"/>
       <c r="E107" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I107" s="21"/>
-      <c r="J107" s="21"/>
-      <c r="L107" s="20"/>
+      <c r="I107" s="23"/>
+      <c r="J107" s="23"/>
+      <c r="L107" s="24"/>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B108" s="23"/>
-      <c r="C108" s="20"/>
-      <c r="D108" s="20"/>
+      <c r="B108" s="22"/>
+      <c r="C108" s="24"/>
+      <c r="D108" s="24"/>
       <c r="E108" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I108" s="21"/>
-      <c r="J108" s="21"/>
-      <c r="L108" s="20"/>
+      <c r="I108" s="23"/>
+      <c r="J108" s="23"/>
+      <c r="L108" s="24"/>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B109" s="23"/>
-      <c r="C109" s="20"/>
-      <c r="D109" s="20"/>
+      <c r="B109" s="22"/>
+      <c r="C109" s="24"/>
+      <c r="D109" s="24"/>
       <c r="E109" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I109" s="21"/>
-      <c r="J109" s="21"/>
-      <c r="L109" s="20"/>
+      <c r="I109" s="23"/>
+      <c r="J109" s="23"/>
+      <c r="L109" s="24"/>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B110" s="23"/>
-      <c r="C110" s="20"/>
-      <c r="D110" s="20"/>
+      <c r="B110" s="22"/>
+      <c r="C110" s="24"/>
+      <c r="D110" s="24"/>
       <c r="E110" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="I110" s="21"/>
-      <c r="J110" s="21"/>
-      <c r="L110" s="20"/>
+      <c r="I110" s="23"/>
+      <c r="J110" s="23"/>
+      <c r="L110" s="24"/>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B111" s="23"/>
-      <c r="C111" s="20"/>
-      <c r="D111" s="20"/>
+      <c r="B111" s="22"/>
+      <c r="C111" s="24"/>
+      <c r="D111" s="24"/>
       <c r="E111" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I111" s="21"/>
-      <c r="J111" s="21"/>
-      <c r="L111" s="20"/>
+      <c r="I111" s="23"/>
+      <c r="J111" s="23"/>
+      <c r="L111" s="24"/>
     </row>
     <row r="112" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="23"/>
+      <c r="B112" s="22"/>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B113" s="23"/>
-      <c r="C113" s="20" t="s">
+      <c r="B113" s="22"/>
+      <c r="C113" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="D113" s="20" t="s">
+      <c r="D113" s="24" t="s">
         <v>107</v>
       </c>
       <c r="E113" s="1" t="s">
@@ -3844,23 +3844,23 @@
       <c r="G113" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="I113" s="21" t="s">
+      <c r="I113" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="J113" s="21" t="s">
+      <c r="J113" s="23" t="s">
         <v>113</v>
       </c>
       <c r="K113" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L113" s="20" t="s">
+      <c r="L113" s="24" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B114" s="23"/>
-      <c r="C114" s="20"/>
-      <c r="D114" s="20"/>
+      <c r="B114" s="22"/>
+      <c r="C114" s="24"/>
+      <c r="D114" s="24"/>
       <c r="E114" s="1" t="s">
         <v>10</v>
       </c>
@@ -3873,14 +3873,14 @@
       <c r="H114" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="I114" s="21"/>
-      <c r="J114" s="21"/>
-      <c r="L114" s="20"/>
+      <c r="I114" s="23"/>
+      <c r="J114" s="23"/>
+      <c r="L114" s="24"/>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B115" s="23"/>
-      <c r="C115" s="20"/>
-      <c r="D115" s="20"/>
+      <c r="B115" s="22"/>
+      <c r="C115" s="24"/>
+      <c r="D115" s="24"/>
       <c r="E115" s="1" t="s">
         <v>30</v>
       </c>
@@ -3890,58 +3890,58 @@
       <c r="G115" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I115" s="21"/>
-      <c r="J115" s="21"/>
-      <c r="L115" s="20"/>
+      <c r="I115" s="23"/>
+      <c r="J115" s="23"/>
+      <c r="L115" s="24"/>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B116" s="23"/>
-      <c r="C116" s="20"/>
-      <c r="D116" s="20"/>
+      <c r="B116" s="22"/>
+      <c r="C116" s="24"/>
+      <c r="D116" s="24"/>
       <c r="E116" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F116" s="1">
         <v>4</v>
       </c>
-      <c r="I116" s="21"/>
-      <c r="J116" s="21"/>
-      <c r="L116" s="20"/>
+      <c r="I116" s="23"/>
+      <c r="J116" s="23"/>
+      <c r="L116" s="24"/>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B117" s="23"/>
-      <c r="C117" s="20"/>
-      <c r="D117" s="20"/>
+      <c r="B117" s="22"/>
+      <c r="C117" s="24"/>
+      <c r="D117" s="24"/>
       <c r="E117" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I117" s="21"/>
-      <c r="J117" s="21"/>
-      <c r="L117" s="20"/>
+      <c r="I117" s="23"/>
+      <c r="J117" s="23"/>
+      <c r="L117" s="24"/>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B118" s="23"/>
-      <c r="C118" s="20"/>
-      <c r="D118" s="20"/>
+      <c r="B118" s="22"/>
+      <c r="C118" s="24"/>
+      <c r="D118" s="24"/>
       <c r="E118" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I118" s="21"/>
-      <c r="J118" s="21"/>
-      <c r="L118" s="20"/>
+      <c r="I118" s="23"/>
+      <c r="J118" s="23"/>
+      <c r="L118" s="24"/>
     </row>
     <row r="119" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="23"/>
+      <c r="B119" s="22"/>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B120" s="23"/>
-      <c r="C120" s="20" t="s">
+      <c r="B120" s="22"/>
+      <c r="C120" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="D120" s="20" t="s">
+      <c r="D120" s="24" t="s">
         <v>115</v>
       </c>
       <c r="E120" s="1" t="s">
@@ -3953,23 +3953,23 @@
       <c r="G120" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I120" s="21" t="s">
+      <c r="I120" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="J120" s="20" t="s">
+      <c r="J120" s="24" t="s">
         <v>124</v>
       </c>
       <c r="K120" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L120" s="21" t="s">
+      <c r="L120" s="23" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B121" s="23"/>
-      <c r="C121" s="20"/>
-      <c r="D121" s="20"/>
+      <c r="B121" s="22"/>
+      <c r="C121" s="24"/>
+      <c r="D121" s="24"/>
       <c r="E121" s="1" t="s">
         <v>10</v>
       </c>
@@ -3979,14 +3979,14 @@
       <c r="G121" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I121" s="21"/>
-      <c r="J121" s="20"/>
-      <c r="L121" s="21"/>
+      <c r="I121" s="23"/>
+      <c r="J121" s="24"/>
+      <c r="L121" s="23"/>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B122" s="23"/>
-      <c r="C122" s="20"/>
-      <c r="D122" s="20"/>
+      <c r="B122" s="22"/>
+      <c r="C122" s="24"/>
+      <c r="D122" s="24"/>
       <c r="E122" s="1" t="s">
         <v>30</v>
       </c>
@@ -3996,55 +3996,55 @@
       <c r="G122" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I122" s="21"/>
-      <c r="J122" s="20"/>
-      <c r="L122" s="21"/>
+      <c r="I122" s="23"/>
+      <c r="J122" s="24"/>
+      <c r="L122" s="23"/>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B123" s="23"/>
-      <c r="C123" s="20"/>
-      <c r="D123" s="20"/>
+      <c r="B123" s="22"/>
+      <c r="C123" s="24"/>
+      <c r="D123" s="24"/>
       <c r="E123" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I123" s="21"/>
-      <c r="J123" s="20"/>
-      <c r="L123" s="21"/>
+      <c r="I123" s="23"/>
+      <c r="J123" s="24"/>
+      <c r="L123" s="23"/>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B124" s="23"/>
-      <c r="C124" s="20"/>
-      <c r="D124" s="20"/>
+      <c r="B124" s="22"/>
+      <c r="C124" s="24"/>
+      <c r="D124" s="24"/>
       <c r="E124" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I124" s="21"/>
-      <c r="J124" s="20"/>
-      <c r="L124" s="21"/>
+      <c r="I124" s="23"/>
+      <c r="J124" s="24"/>
+      <c r="L124" s="23"/>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B125" s="23"/>
-      <c r="C125" s="20"/>
-      <c r="D125" s="20"/>
+      <c r="B125" s="22"/>
+      <c r="C125" s="24"/>
+      <c r="D125" s="24"/>
       <c r="E125" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I125" s="21"/>
-      <c r="J125" s="20"/>
-      <c r="L125" s="21"/>
+      <c r="I125" s="23"/>
+      <c r="J125" s="24"/>
+      <c r="L125" s="23"/>
     </row>
     <row r="126" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="23"/>
+      <c r="B126" s="22"/>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B127" s="23"/>
-      <c r="C127" s="20" t="s">
+      <c r="B127" s="22"/>
+      <c r="C127" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D127" s="20" t="s">
+      <c r="D127" s="24" t="s">
         <v>231</v>
       </c>
       <c r="E127" s="1" t="s">
@@ -4056,23 +4056,23 @@
       <c r="G127" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I127" s="21" t="s">
+      <c r="I127" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="J127" s="21" t="s">
+      <c r="J127" s="23" t="s">
         <v>121</v>
       </c>
       <c r="K127" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L127" s="20" t="s">
+      <c r="L127" s="24" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B128" s="23"/>
-      <c r="C128" s="20"/>
-      <c r="D128" s="20"/>
+      <c r="B128" s="22"/>
+      <c r="C128" s="24"/>
+      <c r="D128" s="24"/>
       <c r="E128" s="1" t="s">
         <v>10</v>
       </c>
@@ -4082,53 +4082,53 @@
       <c r="G128" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="I128" s="21"/>
-      <c r="J128" s="21"/>
-      <c r="L128" s="20"/>
+      <c r="I128" s="23"/>
+      <c r="J128" s="23"/>
+      <c r="L128" s="24"/>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B129" s="23"/>
-      <c r="C129" s="20"/>
-      <c r="D129" s="20"/>
+      <c r="B129" s="22"/>
+      <c r="C129" s="24"/>
+      <c r="D129" s="24"/>
       <c r="E129" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I129" s="21"/>
-      <c r="J129" s="21"/>
-      <c r="L129" s="20"/>
+      <c r="I129" s="23"/>
+      <c r="J129" s="23"/>
+      <c r="L129" s="24"/>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B130" s="23"/>
-      <c r="C130" s="20"/>
-      <c r="D130" s="20"/>
+      <c r="B130" s="22"/>
+      <c r="C130" s="24"/>
+      <c r="D130" s="24"/>
       <c r="E130" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I130" s="21"/>
-      <c r="J130" s="21"/>
-      <c r="L130" s="20"/>
+      <c r="I130" s="23"/>
+      <c r="J130" s="23"/>
+      <c r="L130" s="24"/>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B131" s="23"/>
-      <c r="C131" s="20"/>
-      <c r="D131" s="20"/>
+      <c r="B131" s="22"/>
+      <c r="C131" s="24"/>
+      <c r="D131" s="24"/>
       <c r="E131" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I131" s="21"/>
-      <c r="J131" s="21"/>
-      <c r="L131" s="20"/>
+      <c r="I131" s="23"/>
+      <c r="J131" s="23"/>
+      <c r="L131" s="24"/>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B132" s="23"/>
-      <c r="C132" s="20"/>
-      <c r="D132" s="20"/>
+      <c r="B132" s="22"/>
+      <c r="C132" s="24"/>
+      <c r="D132" s="24"/>
       <c r="E132" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I132" s="21"/>
-      <c r="J132" s="21"/>
-      <c r="L132" s="20"/>
+      <c r="I132" s="23"/>
+      <c r="J132" s="23"/>
+      <c r="L132" s="24"/>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C133" s="3"/>
@@ -4140,13 +4140,13 @@
       <c r="A137" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B137" s="23" t="s">
+      <c r="B137" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="C137" s="21" t="s">
+      <c r="C137" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="D137" s="21" t="s">
+      <c r="D137" s="23" t="s">
         <v>145</v>
       </c>
       <c r="E137" s="1" t="s">
@@ -4158,20 +4158,20 @@
       <c r="G137" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I137" s="21" t="s">
+      <c r="I137" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="J137" s="21" t="s">
+      <c r="J137" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="K137" s="20" t="s">
+      <c r="K137" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="138" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="23"/>
-      <c r="C138" s="21"/>
-      <c r="D138" s="21"/>
+      <c r="B138" s="22"/>
+      <c r="C138" s="23"/>
+      <c r="D138" s="23"/>
       <c r="E138" s="1" t="s">
         <v>10</v>
       </c>
@@ -4181,14 +4181,14 @@
       <c r="G138" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="I138" s="21"/>
-      <c r="J138" s="21"/>
-      <c r="K138" s="20"/>
+      <c r="I138" s="23"/>
+      <c r="J138" s="23"/>
+      <c r="K138" s="24"/>
     </row>
     <row r="139" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="23"/>
-      <c r="C139" s="21"/>
-      <c r="D139" s="21"/>
+      <c r="B139" s="22"/>
+      <c r="C139" s="23"/>
+      <c r="D139" s="23"/>
       <c r="E139" s="1" t="s">
         <v>30</v>
       </c>
@@ -4198,13 +4198,13 @@
       <c r="G139" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="I139" s="21"/>
-      <c r="J139" s="21"/>
+      <c r="I139" s="23"/>
+      <c r="J139" s="23"/>
     </row>
     <row r="140" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="23"/>
-      <c r="C140" s="21"/>
-      <c r="D140" s="21"/>
+      <c r="B140" s="22"/>
+      <c r="C140" s="23"/>
+      <c r="D140" s="23"/>
       <c r="E140" s="1" t="s">
         <v>32</v>
       </c>
@@ -4214,13 +4214,13 @@
       <c r="G140" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I140" s="21"/>
-      <c r="J140" s="21"/>
+      <c r="I140" s="23"/>
+      <c r="J140" s="23"/>
     </row>
     <row r="141" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="23"/>
-      <c r="C141" s="21"/>
-      <c r="D141" s="21"/>
+      <c r="B141" s="22"/>
+      <c r="C141" s="23"/>
+      <c r="D141" s="23"/>
       <c r="E141" s="1" t="s">
         <v>131</v>
       </c>
@@ -4230,13 +4230,13 @@
       <c r="G141" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I141" s="21"/>
-      <c r="J141" s="21"/>
+      <c r="I141" s="23"/>
+      <c r="J141" s="23"/>
     </row>
     <row r="142" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="23"/>
-      <c r="C142" s="21"/>
-      <c r="D142" s="21"/>
+      <c r="B142" s="22"/>
+      <c r="C142" s="23"/>
+      <c r="D142" s="23"/>
       <c r="E142" s="1" t="s">
         <v>38</v>
       </c>
@@ -4246,11 +4246,11 @@
       <c r="G142" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I142" s="21"/>
-      <c r="J142" s="21"/>
+      <c r="I142" s="23"/>
+      <c r="J142" s="23"/>
     </row>
     <row r="143" spans="1:12" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="23"/>
+      <c r="B143" s="22"/>
       <c r="C143" s="9"/>
       <c r="D143" s="9"/>
     </row>
@@ -4258,11 +4258,11 @@
       <c r="A144" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B144" s="23"/>
-      <c r="C144" s="20" t="s">
+      <c r="B144" s="22"/>
+      <c r="C144" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="D144" s="21" t="s">
+      <c r="D144" s="23" t="s">
         <v>162</v>
       </c>
       <c r="E144" s="1" t="s">
@@ -4274,20 +4274,20 @@
       <c r="G144" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="I144" s="21" t="s">
+      <c r="I144" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="J144" s="21" t="s">
+      <c r="J144" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="K144" s="20" t="s">
+      <c r="K144" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="23"/>
-      <c r="C145" s="20"/>
-      <c r="D145" s="21"/>
+      <c r="B145" s="22"/>
+      <c r="C145" s="24"/>
+      <c r="D145" s="23"/>
       <c r="E145" s="1" t="s">
         <v>10</v>
       </c>
@@ -4300,14 +4300,14 @@
       <c r="H145" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I145" s="21"/>
-      <c r="J145" s="21"/>
-      <c r="K145" s="20"/>
+      <c r="I145" s="23"/>
+      <c r="J145" s="23"/>
+      <c r="K145" s="24"/>
     </row>
     <row r="146" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="23"/>
-      <c r="C146" s="20"/>
-      <c r="D146" s="21"/>
+      <c r="B146" s="22"/>
+      <c r="C146" s="24"/>
+      <c r="D146" s="23"/>
       <c r="E146" s="1" t="s">
         <v>30</v>
       </c>
@@ -4317,51 +4317,51 @@
       <c r="G146" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I146" s="21"/>
-      <c r="J146" s="21"/>
+      <c r="I146" s="23"/>
+      <c r="J146" s="23"/>
     </row>
     <row r="147" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="23"/>
-      <c r="C147" s="20"/>
-      <c r="D147" s="21"/>
+      <c r="B147" s="22"/>
+      <c r="C147" s="24"/>
+      <c r="D147" s="23"/>
       <c r="E147" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I147" s="21"/>
-      <c r="J147" s="21"/>
+      <c r="I147" s="23"/>
+      <c r="J147" s="23"/>
     </row>
     <row r="148" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="23"/>
-      <c r="C148" s="20"/>
-      <c r="D148" s="21"/>
+      <c r="B148" s="22"/>
+      <c r="C148" s="24"/>
+      <c r="D148" s="23"/>
       <c r="E148" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I148" s="21"/>
-      <c r="J148" s="21"/>
+      <c r="I148" s="23"/>
+      <c r="J148" s="23"/>
     </row>
     <row r="149" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="23"/>
-      <c r="C149" s="20"/>
-      <c r="D149" s="21"/>
+      <c r="B149" s="22"/>
+      <c r="C149" s="24"/>
+      <c r="D149" s="23"/>
       <c r="E149" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I149" s="21"/>
-      <c r="J149" s="21"/>
+      <c r="I149" s="23"/>
+      <c r="J149" s="23"/>
     </row>
     <row r="150" spans="1:12" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="23"/>
+      <c r="B150" s="22"/>
     </row>
     <row r="151" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B151" s="23"/>
-      <c r="C151" s="21" t="s">
+      <c r="B151" s="22"/>
+      <c r="C151" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="D151" s="21" t="s">
+      <c r="D151" s="23" t="s">
         <v>163</v>
       </c>
       <c r="E151" s="1" t="s">
@@ -4376,23 +4376,23 @@
       <c r="H151" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I151" s="20" t="s">
+      <c r="I151" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="J151" s="20" t="s">
+      <c r="J151" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="K151" s="20" t="s">
+      <c r="K151" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L151" s="20" t="s">
+      <c r="L151" s="24" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="152" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="23"/>
-      <c r="C152" s="21"/>
-      <c r="D152" s="21"/>
+      <c r="B152" s="22"/>
+      <c r="C152" s="23"/>
+      <c r="D152" s="23"/>
       <c r="E152" s="1" t="s">
         <v>10</v>
       </c>
@@ -4402,15 +4402,15 @@
       <c r="G152" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I152" s="20"/>
-      <c r="J152" s="20"/>
-      <c r="K152" s="20"/>
-      <c r="L152" s="20"/>
+      <c r="I152" s="24"/>
+      <c r="J152" s="24"/>
+      <c r="K152" s="24"/>
+      <c r="L152" s="24"/>
     </row>
     <row r="153" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="23"/>
-      <c r="C153" s="21"/>
-      <c r="D153" s="21"/>
+      <c r="B153" s="22"/>
+      <c r="C153" s="23"/>
+      <c r="D153" s="23"/>
       <c r="E153" s="1" t="s">
         <v>30</v>
       </c>
@@ -4420,44 +4420,44 @@
       <c r="G153" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I153" s="20"/>
-      <c r="J153" s="20"/>
-      <c r="L153" s="20"/>
+      <c r="I153" s="24"/>
+      <c r="J153" s="24"/>
+      <c r="L153" s="24"/>
     </row>
     <row r="154" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="23"/>
-      <c r="C154" s="21"/>
-      <c r="D154" s="21"/>
+      <c r="B154" s="22"/>
+      <c r="C154" s="23"/>
+      <c r="D154" s="23"/>
       <c r="E154" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I154" s="20"/>
-      <c r="J154" s="20"/>
-      <c r="L154" s="20"/>
+      <c r="I154" s="24"/>
+      <c r="J154" s="24"/>
+      <c r="L154" s="24"/>
     </row>
     <row r="155" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="23"/>
-      <c r="C155" s="21"/>
-      <c r="D155" s="21"/>
+      <c r="B155" s="22"/>
+      <c r="C155" s="23"/>
+      <c r="D155" s="23"/>
       <c r="E155" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I155" s="20"/>
-      <c r="J155" s="20"/>
-      <c r="L155" s="20"/>
+      <c r="I155" s="24"/>
+      <c r="J155" s="24"/>
+      <c r="L155" s="24"/>
     </row>
     <row r="156" spans="1:12" s="6" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="23"/>
+      <c r="B156" s="22"/>
     </row>
     <row r="157" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B157" s="23"/>
-      <c r="C157" s="20" t="s">
+      <c r="B157" s="22"/>
+      <c r="C157" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="D157" s="20" t="s">
+      <c r="D157" s="24" t="s">
         <v>157</v>
       </c>
       <c r="E157" s="1" t="s">
@@ -4469,23 +4469,23 @@
       <c r="G157" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H157" s="21" t="s">
+      <c r="H157" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="I157" s="21" t="s">
+      <c r="I157" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="J157" s="21" t="s">
+      <c r="J157" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="K157" s="20" t="s">
+      <c r="K157" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="158" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="23"/>
-      <c r="C158" s="20"/>
-      <c r="D158" s="20"/>
+      <c r="B158" s="22"/>
+      <c r="C158" s="24"/>
+      <c r="D158" s="24"/>
       <c r="E158" s="1" t="s">
         <v>10</v>
       </c>
@@ -4495,15 +4495,15 @@
       <c r="G158" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H158" s="21"/>
-      <c r="I158" s="21"/>
-      <c r="J158" s="21"/>
-      <c r="K158" s="20"/>
+      <c r="H158" s="23"/>
+      <c r="I158" s="23"/>
+      <c r="J158" s="23"/>
+      <c r="K158" s="24"/>
     </row>
     <row r="159" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="23"/>
-      <c r="C159" s="20"/>
-      <c r="D159" s="20"/>
+      <c r="B159" s="22"/>
+      <c r="C159" s="24"/>
+      <c r="D159" s="24"/>
       <c r="E159" s="1" t="s">
         <v>30</v>
       </c>
@@ -4513,14 +4513,14 @@
       <c r="G159" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H159" s="21"/>
-      <c r="I159" s="21"/>
-      <c r="J159" s="21"/>
+      <c r="H159" s="23"/>
+      <c r="I159" s="23"/>
+      <c r="J159" s="23"/>
     </row>
     <row r="160" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="23"/>
-      <c r="C160" s="20"/>
-      <c r="D160" s="20"/>
+      <c r="B160" s="22"/>
+      <c r="C160" s="24"/>
+      <c r="D160" s="24"/>
       <c r="E160" s="1" t="s">
         <v>32</v>
       </c>
@@ -4530,14 +4530,14 @@
       <c r="G160" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H160" s="21"/>
-      <c r="I160" s="21"/>
-      <c r="J160" s="21"/>
+      <c r="H160" s="23"/>
+      <c r="I160" s="23"/>
+      <c r="J160" s="23"/>
     </row>
     <row r="161" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="23"/>
-      <c r="C161" s="20"/>
-      <c r="D161" s="20"/>
+      <c r="B161" s="22"/>
+      <c r="C161" s="24"/>
+      <c r="D161" s="24"/>
       <c r="E161" s="1" t="s">
         <v>154</v>
       </c>
@@ -4547,16 +4547,16 @@
       <c r="G161" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="H161" s="21" t="s">
+      <c r="H161" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="I161" s="21"/>
-      <c r="J161" s="21"/>
+      <c r="I161" s="23"/>
+      <c r="J161" s="23"/>
     </row>
     <row r="162" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="23"/>
-      <c r="C162" s="20"/>
-      <c r="D162" s="20"/>
+      <c r="B162" s="22"/>
+      <c r="C162" s="24"/>
+      <c r="D162" s="24"/>
       <c r="E162" s="1" t="s">
         <v>38</v>
       </c>
@@ -4566,50 +4566,50 @@
       <c r="G162" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H162" s="21"/>
-      <c r="I162" s="21"/>
-      <c r="J162" s="21"/>
+      <c r="H162" s="23"/>
+      <c r="I162" s="23"/>
+      <c r="J162" s="23"/>
     </row>
     <row r="163" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="23"/>
-      <c r="C163" s="20"/>
-      <c r="D163" s="20"/>
+      <c r="B163" s="22"/>
+      <c r="C163" s="24"/>
+      <c r="D163" s="24"/>
       <c r="F163" s="1">
         <v>7</v>
       </c>
       <c r="G163" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H163" s="21"/>
-      <c r="I163" s="21"/>
-      <c r="J163" s="21"/>
+      <c r="H163" s="23"/>
+      <c r="I163" s="23"/>
+      <c r="J163" s="23"/>
     </row>
     <row r="164" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="23"/>
-      <c r="C164" s="20"/>
-      <c r="D164" s="20"/>
+      <c r="B164" s="22"/>
+      <c r="C164" s="24"/>
+      <c r="D164" s="24"/>
       <c r="F164" s="1">
         <v>8</v>
       </c>
       <c r="G164" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H164" s="21"/>
-      <c r="I164" s="21"/>
-      <c r="J164" s="21"/>
+      <c r="H164" s="23"/>
+      <c r="I164" s="23"/>
+      <c r="J164" s="23"/>
     </row>
     <row r="165" spans="1:12" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="23"/>
+      <c r="B165" s="22"/>
     </row>
     <row r="166" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B166" s="23"/>
-      <c r="C166" s="20" t="s">
+      <c r="B166" s="22"/>
+      <c r="C166" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="D166" s="20" t="s">
+      <c r="D166" s="24" t="s">
         <v>82</v>
       </c>
       <c r="E166" s="1" t="s">
@@ -4624,23 +4624,23 @@
       <c r="H166" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I166" s="20" t="s">
+      <c r="I166" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="J166" s="20" t="s">
+      <c r="J166" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="K166" s="20" t="s">
+      <c r="K166" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L166" s="22" t="s">
+      <c r="L166" s="26" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="167" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B167" s="23"/>
-      <c r="C167" s="20"/>
-      <c r="D167" s="20"/>
+      <c r="B167" s="22"/>
+      <c r="C167" s="24"/>
+      <c r="D167" s="24"/>
       <c r="E167" s="1" t="s">
         <v>10</v>
       </c>
@@ -4653,15 +4653,15 @@
       <c r="H167" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I167" s="20"/>
-      <c r="J167" s="20"/>
-      <c r="K167" s="20"/>
-      <c r="L167" s="22"/>
+      <c r="I167" s="24"/>
+      <c r="J167" s="24"/>
+      <c r="K167" s="24"/>
+      <c r="L167" s="26"/>
     </row>
     <row r="168" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B168" s="23"/>
-      <c r="C168" s="20"/>
-      <c r="D168" s="20"/>
+      <c r="B168" s="22"/>
+      <c r="C168" s="24"/>
+      <c r="D168" s="24"/>
       <c r="E168" s="1" t="s">
         <v>30</v>
       </c>
@@ -4674,53 +4674,53 @@
       <c r="H168" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I168" s="20"/>
-      <c r="J168" s="20"/>
-      <c r="L168" s="22"/>
+      <c r="I168" s="24"/>
+      <c r="J168" s="24"/>
+      <c r="L168" s="26"/>
     </row>
     <row r="169" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B169" s="23"/>
-      <c r="C169" s="20"/>
-      <c r="D169" s="20"/>
+      <c r="B169" s="22"/>
+      <c r="C169" s="24"/>
+      <c r="D169" s="24"/>
       <c r="E169" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I169" s="20"/>
-      <c r="J169" s="20"/>
-      <c r="L169" s="22"/>
+      <c r="I169" s="24"/>
+      <c r="J169" s="24"/>
+      <c r="L169" s="26"/>
     </row>
     <row r="170" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B170" s="23"/>
-      <c r="C170" s="20"/>
-      <c r="D170" s="20"/>
+      <c r="B170" s="22"/>
+      <c r="C170" s="24"/>
+      <c r="D170" s="24"/>
       <c r="E170" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I170" s="20"/>
-      <c r="J170" s="20"/>
-      <c r="L170" s="22"/>
+      <c r="I170" s="24"/>
+      <c r="J170" s="24"/>
+      <c r="L170" s="26"/>
     </row>
     <row r="171" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B171" s="23"/>
-      <c r="C171" s="20"/>
-      <c r="D171" s="20"/>
+      <c r="B171" s="22"/>
+      <c r="C171" s="24"/>
+      <c r="D171" s="24"/>
       <c r="E171" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I171" s="20"/>
-      <c r="J171" s="20"/>
-      <c r="L171" s="22"/>
+      <c r="I171" s="24"/>
+      <c r="J171" s="24"/>
+      <c r="L171" s="26"/>
     </row>
     <row r="172" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="23"/>
-      <c r="C172" s="20"/>
-      <c r="D172" s="20"/>
+      <c r="B172" s="22"/>
+      <c r="C172" s="24"/>
+      <c r="D172" s="24"/>
       <c r="E172" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I172" s="20"/>
-      <c r="J172" s="20"/>
-      <c r="L172" s="22"/>
+      <c r="I172" s="24"/>
+      <c r="J172" s="24"/>
+      <c r="L172" s="26"/>
     </row>
     <row r="174" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="175" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -4728,13 +4728,13 @@
       <c r="A177" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B177" s="23" t="s">
+      <c r="B177" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="C177" s="20" t="s">
+      <c r="C177" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="D177" s="20" t="s">
+      <c r="D177" s="24" t="s">
         <v>198</v>
       </c>
       <c r="E177" s="10" t="s">
@@ -4747,10 +4747,10 @@
         <v>182</v>
       </c>
       <c r="H177" s="10"/>
-      <c r="I177" s="21" t="s">
+      <c r="I177" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="J177" s="21" t="s">
+      <c r="J177" s="23" t="s">
         <v>184</v>
       </c>
       <c r="K177" s="10" t="s">
@@ -4758,9 +4758,9 @@
       </c>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B178" s="23"/>
-      <c r="C178" s="20"/>
-      <c r="D178" s="20"/>
+      <c r="B178" s="22"/>
+      <c r="C178" s="24"/>
+      <c r="D178" s="24"/>
       <c r="E178" s="10" t="s">
         <v>10</v>
       </c>
@@ -4771,14 +4771,14 @@
         <v>183</v>
       </c>
       <c r="H178" s="10"/>
-      <c r="I178" s="21"/>
-      <c r="J178" s="21"/>
+      <c r="I178" s="23"/>
+      <c r="J178" s="23"/>
       <c r="K178" s="10"/>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B179" s="23"/>
-      <c r="C179" s="20"/>
-      <c r="D179" s="20"/>
+      <c r="B179" s="22"/>
+      <c r="C179" s="24"/>
+      <c r="D179" s="24"/>
       <c r="E179" s="10" t="s">
         <v>30</v>
       </c>
@@ -4789,14 +4789,14 @@
         <v>192</v>
       </c>
       <c r="H179" s="10"/>
-      <c r="I179" s="21"/>
-      <c r="J179" s="21"/>
+      <c r="I179" s="23"/>
+      <c r="J179" s="23"/>
       <c r="K179" s="10"/>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B180" s="23"/>
-      <c r="C180" s="20"/>
-      <c r="D180" s="20"/>
+      <c r="B180" s="22"/>
+      <c r="C180" s="24"/>
+      <c r="D180" s="24"/>
       <c r="E180" s="10" t="s">
         <v>32</v>
       </c>
@@ -4807,14 +4807,14 @@
         <v>230</v>
       </c>
       <c r="H180" s="10"/>
-      <c r="I180" s="21"/>
-      <c r="J180" s="21"/>
+      <c r="I180" s="23"/>
+      <c r="J180" s="23"/>
       <c r="K180" s="10"/>
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B181" s="23"/>
-      <c r="C181" s="20"/>
-      <c r="D181" s="20"/>
+      <c r="B181" s="22"/>
+      <c r="C181" s="24"/>
+      <c r="D181" s="24"/>
       <c r="E181" s="10" t="s">
         <v>199</v>
       </c>
@@ -4825,36 +4825,36 @@
         <v>186</v>
       </c>
       <c r="H181" s="10"/>
-      <c r="I181" s="21"/>
-      <c r="J181" s="21"/>
+      <c r="I181" s="23"/>
+      <c r="J181" s="23"/>
       <c r="K181" s="10"/>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B182" s="23"/>
-      <c r="C182" s="20"/>
-      <c r="D182" s="20"/>
+      <c r="B182" s="22"/>
+      <c r="C182" s="24"/>
+      <c r="D182" s="24"/>
       <c r="E182" s="10" t="s">
         <v>38</v>
       </c>
       <c r="F182" s="10"/>
       <c r="G182" s="10"/>
       <c r="H182" s="10"/>
-      <c r="I182" s="21"/>
-      <c r="J182" s="21"/>
+      <c r="I182" s="23"/>
+      <c r="J182" s="23"/>
       <c r="K182" s="10"/>
     </row>
     <row r="183" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B183" s="23"/>
+      <c r="B183" s="22"/>
     </row>
     <row r="184" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B184" s="23"/>
-      <c r="C184" s="20" t="s">
+      <c r="B184" s="22"/>
+      <c r="C184" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="D184" s="20" t="s">
+      <c r="D184" s="24" t="s">
         <v>188</v>
       </c>
       <c r="E184" s="10" t="s">
@@ -4867,10 +4867,10 @@
         <v>182</v>
       </c>
       <c r="H184" s="1"/>
-      <c r="I184" s="21" t="s">
+      <c r="I184" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="J184" s="21" t="s">
+      <c r="J184" s="23" t="s">
         <v>184</v>
       </c>
       <c r="K184" s="1" t="s">
@@ -4878,9 +4878,9 @@
       </c>
     </row>
     <row r="185" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B185" s="23"/>
-      <c r="C185" s="20"/>
-      <c r="D185" s="20"/>
+      <c r="B185" s="22"/>
+      <c r="C185" s="24"/>
+      <c r="D185" s="24"/>
       <c r="E185" s="10" t="s">
         <v>10</v>
       </c>
@@ -4891,14 +4891,14 @@
         <v>183</v>
       </c>
       <c r="H185" s="1"/>
-      <c r="I185" s="21"/>
-      <c r="J185" s="21"/>
+      <c r="I185" s="23"/>
+      <c r="J185" s="23"/>
       <c r="K185" s="1"/>
     </row>
     <row r="186" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B186" s="23"/>
-      <c r="C186" s="20"/>
-      <c r="D186" s="20"/>
+      <c r="B186" s="22"/>
+      <c r="C186" s="24"/>
+      <c r="D186" s="24"/>
       <c r="E186" s="10" t="s">
         <v>30</v>
       </c>
@@ -4909,14 +4909,14 @@
         <v>192</v>
       </c>
       <c r="H186" s="1"/>
-      <c r="I186" s="21"/>
-      <c r="J186" s="21"/>
+      <c r="I186" s="23"/>
+      <c r="J186" s="23"/>
       <c r="K186" s="1"/>
     </row>
     <row r="187" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B187" s="23"/>
-      <c r="C187" s="20"/>
-      <c r="D187" s="20"/>
+      <c r="B187" s="22"/>
+      <c r="C187" s="24"/>
+      <c r="D187" s="24"/>
       <c r="E187" s="10" t="s">
         <v>32</v>
       </c>
@@ -4927,14 +4927,14 @@
         <v>185</v>
       </c>
       <c r="H187" s="1"/>
-      <c r="I187" s="21"/>
-      <c r="J187" s="21"/>
+      <c r="I187" s="23"/>
+      <c r="J187" s="23"/>
       <c r="K187" s="1"/>
     </row>
     <row r="188" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B188" s="23"/>
-      <c r="C188" s="20"/>
-      <c r="D188" s="20"/>
+      <c r="B188" s="22"/>
+      <c r="C188" s="24"/>
+      <c r="D188" s="24"/>
       <c r="E188" s="10" t="s">
         <v>181</v>
       </c>
@@ -4945,14 +4945,14 @@
         <v>186</v>
       </c>
       <c r="H188" s="1"/>
-      <c r="I188" s="21"/>
-      <c r="J188" s="21"/>
+      <c r="I188" s="23"/>
+      <c r="J188" s="23"/>
       <c r="K188" s="1"/>
     </row>
     <row r="189" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B189" s="23"/>
-      <c r="C189" s="20"/>
-      <c r="D189" s="20"/>
+      <c r="B189" s="22"/>
+      <c r="C189" s="24"/>
+      <c r="D189" s="24"/>
       <c r="E189" s="10" t="s">
         <v>38</v>
       </c>
@@ -4963,22 +4963,22 @@
         <v>190</v>
       </c>
       <c r="H189" s="1"/>
-      <c r="I189" s="21"/>
-      <c r="J189" s="21"/>
+      <c r="I189" s="23"/>
+      <c r="J189" s="23"/>
       <c r="K189" s="1"/>
     </row>
     <row r="190" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B190" s="23"/>
+      <c r="B190" s="22"/>
     </row>
     <row r="191" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="B191" s="23"/>
-      <c r="C191" s="20" t="s">
+      <c r="B191" s="22"/>
+      <c r="C191" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="D191" s="20" t="s">
+      <c r="D191" s="24" t="s">
         <v>189</v>
       </c>
       <c r="E191" s="10" t="s">
@@ -4990,10 +4990,10 @@
       <c r="G191" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="I191" s="21" t="s">
+      <c r="I191" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="J191" s="21" t="s">
+      <c r="J191" s="23" t="s">
         <v>184</v>
       </c>
       <c r="K191" s="10" t="s">
@@ -5001,9 +5001,9 @@
       </c>
     </row>
     <row r="192" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B192" s="23"/>
-      <c r="C192" s="20"/>
-      <c r="D192" s="20"/>
+      <c r="B192" s="22"/>
+      <c r="C192" s="24"/>
+      <c r="D192" s="24"/>
       <c r="E192" s="10" t="s">
         <v>10</v>
       </c>
@@ -5013,13 +5013,13 @@
       <c r="G192" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="I192" s="21"/>
-      <c r="J192" s="21"/>
+      <c r="I192" s="23"/>
+      <c r="J192" s="23"/>
     </row>
     <row r="193" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B193" s="23"/>
-      <c r="C193" s="20"/>
-      <c r="D193" s="20"/>
+      <c r="B193" s="22"/>
+      <c r="C193" s="24"/>
+      <c r="D193" s="24"/>
       <c r="E193" s="10" t="s">
         <v>30</v>
       </c>
@@ -5029,13 +5029,13 @@
       <c r="G193" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="I193" s="21"/>
-      <c r="J193" s="21"/>
+      <c r="I193" s="23"/>
+      <c r="J193" s="23"/>
     </row>
     <row r="194" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B194" s="23"/>
-      <c r="C194" s="20"/>
-      <c r="D194" s="20"/>
+      <c r="B194" s="22"/>
+      <c r="C194" s="24"/>
+      <c r="D194" s="24"/>
       <c r="E194" s="10" t="s">
         <v>32</v>
       </c>
@@ -5045,13 +5045,13 @@
       <c r="G194" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="I194" s="21"/>
-      <c r="J194" s="21"/>
+      <c r="I194" s="23"/>
+      <c r="J194" s="23"/>
     </row>
     <row r="195" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B195" s="23"/>
-      <c r="C195" s="20"/>
-      <c r="D195" s="20"/>
+      <c r="B195" s="22"/>
+      <c r="C195" s="24"/>
+      <c r="D195" s="24"/>
       <c r="E195" s="10" t="s">
         <v>69</v>
       </c>
@@ -5061,13 +5061,13 @@
       <c r="G195" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="I195" s="21"/>
-      <c r="J195" s="21"/>
+      <c r="I195" s="23"/>
+      <c r="J195" s="23"/>
     </row>
     <row r="196" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B196" s="23"/>
-      <c r="C196" s="20"/>
-      <c r="D196" s="20"/>
+      <c r="B196" s="22"/>
+      <c r="C196" s="24"/>
+      <c r="D196" s="24"/>
       <c r="E196" s="10" t="s">
         <v>38</v>
       </c>
@@ -5077,21 +5077,21 @@
       <c r="G196" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="I196" s="21"/>
-      <c r="J196" s="21"/>
+      <c r="I196" s="23"/>
+      <c r="J196" s="23"/>
     </row>
     <row r="197" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B197" s="23"/>
+      <c r="B197" s="22"/>
     </row>
     <row r="198" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="B198" s="23"/>
-      <c r="C198" s="20" t="s">
+      <c r="B198" s="22"/>
+      <c r="C198" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="D198" s="20" t="s">
+      <c r="D198" s="24" t="s">
         <v>195</v>
       </c>
       <c r="E198" s="10" t="s">
@@ -5103,10 +5103,10 @@
       <c r="G198" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="I198" s="21" t="s">
+      <c r="I198" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="J198" s="21" t="s">
+      <c r="J198" s="23" t="s">
         <v>184</v>
       </c>
       <c r="K198" s="10" t="s">
@@ -5114,9 +5114,9 @@
       </c>
     </row>
     <row r="199" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B199" s="23"/>
-      <c r="C199" s="20"/>
-      <c r="D199" s="20"/>
+      <c r="B199" s="22"/>
+      <c r="C199" s="24"/>
+      <c r="D199" s="24"/>
       <c r="E199" s="10" t="s">
         <v>10</v>
       </c>
@@ -5126,13 +5126,13 @@
       <c r="G199" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="I199" s="21"/>
-      <c r="J199" s="21"/>
+      <c r="I199" s="23"/>
+      <c r="J199" s="23"/>
     </row>
     <row r="200" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B200" s="23"/>
-      <c r="C200" s="20"/>
-      <c r="D200" s="20"/>
+      <c r="B200" s="22"/>
+      <c r="C200" s="24"/>
+      <c r="D200" s="24"/>
       <c r="E200" s="10" t="s">
         <v>30</v>
       </c>
@@ -5142,13 +5142,13 @@
       <c r="G200" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="I200" s="21"/>
-      <c r="J200" s="21"/>
+      <c r="I200" s="23"/>
+      <c r="J200" s="23"/>
     </row>
     <row r="201" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B201" s="23"/>
-      <c r="C201" s="20"/>
-      <c r="D201" s="20"/>
+      <c r="B201" s="22"/>
+      <c r="C201" s="24"/>
+      <c r="D201" s="24"/>
       <c r="E201" s="10" t="s">
         <v>32</v>
       </c>
@@ -5158,13 +5158,13 @@
       <c r="G201" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="I201" s="21"/>
-      <c r="J201" s="21"/>
+      <c r="I201" s="23"/>
+      <c r="J201" s="23"/>
     </row>
     <row r="202" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B202" s="23"/>
-      <c r="C202" s="20"/>
-      <c r="D202" s="20"/>
+      <c r="B202" s="22"/>
+      <c r="C202" s="24"/>
+      <c r="D202" s="24"/>
       <c r="E202" s="10" t="s">
         <v>91</v>
       </c>
@@ -5174,13 +5174,13 @@
       <c r="G202" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="I202" s="21"/>
-      <c r="J202" s="21"/>
+      <c r="I202" s="23"/>
+      <c r="J202" s="23"/>
     </row>
     <row r="203" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B203" s="23"/>
-      <c r="C203" s="20"/>
-      <c r="D203" s="20"/>
+      <c r="B203" s="22"/>
+      <c r="C203" s="24"/>
+      <c r="D203" s="24"/>
       <c r="E203" s="10" t="s">
         <v>38</v>
       </c>
@@ -5190,21 +5190,21 @@
       <c r="G203" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="I203" s="21"/>
-      <c r="J203" s="21"/>
+      <c r="I203" s="23"/>
+      <c r="J203" s="23"/>
     </row>
     <row r="204" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B204" s="23"/>
+      <c r="B204" s="22"/>
     </row>
     <row r="205" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B205" s="23"/>
-      <c r="C205" s="20" t="s">
+      <c r="B205" s="22"/>
+      <c r="C205" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="D205" s="20" t="s">
+      <c r="D205" s="24" t="s">
         <v>196</v>
       </c>
       <c r="E205" s="10" t="s">
@@ -5216,10 +5216,10 @@
       <c r="G205" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="I205" s="21" t="s">
+      <c r="I205" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="J205" s="21" t="s">
+      <c r="J205" s="23" t="s">
         <v>184</v>
       </c>
       <c r="K205" s="10" t="s">
@@ -5227,9 +5227,9 @@
       </c>
     </row>
     <row r="206" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B206" s="23"/>
-      <c r="C206" s="20"/>
-      <c r="D206" s="20"/>
+      <c r="B206" s="22"/>
+      <c r="C206" s="24"/>
+      <c r="D206" s="24"/>
       <c r="E206" s="10" t="s">
         <v>10</v>
       </c>
@@ -5239,13 +5239,13 @@
       <c r="G206" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="I206" s="21"/>
-      <c r="J206" s="21"/>
+      <c r="I206" s="23"/>
+      <c r="J206" s="23"/>
     </row>
     <row r="207" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B207" s="23"/>
-      <c r="C207" s="20"/>
-      <c r="D207" s="20"/>
+      <c r="B207" s="22"/>
+      <c r="C207" s="24"/>
+      <c r="D207" s="24"/>
       <c r="E207" s="10" t="s">
         <v>30</v>
       </c>
@@ -5255,13 +5255,13 @@
       <c r="G207" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="I207" s="21"/>
-      <c r="J207" s="21"/>
+      <c r="I207" s="23"/>
+      <c r="J207" s="23"/>
     </row>
     <row r="208" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B208" s="23"/>
-      <c r="C208" s="20"/>
-      <c r="D208" s="20"/>
+      <c r="B208" s="22"/>
+      <c r="C208" s="24"/>
+      <c r="D208" s="24"/>
       <c r="E208" s="10" t="s">
         <v>32</v>
       </c>
@@ -5271,13 +5271,13 @@
       <c r="G208" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="I208" s="21"/>
-      <c r="J208" s="21"/>
+      <c r="I208" s="23"/>
+      <c r="J208" s="23"/>
     </row>
     <row r="209" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B209" s="23"/>
-      <c r="C209" s="20"/>
-      <c r="D209" s="20"/>
+      <c r="B209" s="22"/>
+      <c r="C209" s="24"/>
+      <c r="D209" s="24"/>
       <c r="E209" s="10" t="s">
         <v>131</v>
       </c>
@@ -5287,13 +5287,13 @@
       <c r="G209" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="I209" s="21"/>
-      <c r="J209" s="21"/>
+      <c r="I209" s="23"/>
+      <c r="J209" s="23"/>
     </row>
     <row r="210" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B210" s="23"/>
-      <c r="C210" s="20"/>
-      <c r="D210" s="20"/>
+      <c r="B210" s="22"/>
+      <c r="C210" s="24"/>
+      <c r="D210" s="24"/>
       <c r="E210" s="10" t="s">
         <v>38</v>
       </c>
@@ -5303,8 +5303,8 @@
       <c r="G210" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="I210" s="21"/>
-      <c r="J210" s="21"/>
+      <c r="I210" s="23"/>
+      <c r="J210" s="23"/>
     </row>
     <row r="212" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="213" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -5313,13 +5313,13 @@
       <c r="A215" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B215" s="23" t="s">
+      <c r="B215" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="C215" s="20" t="s">
+      <c r="C215" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D215" s="20" t="s">
+      <c r="D215" s="24" t="s">
         <v>205</v>
       </c>
       <c r="E215" s="10" t="s">
@@ -5328,13 +5328,13 @@
       <c r="F215" s="10">
         <v>1</v>
       </c>
-      <c r="G215" s="21" t="s">
+      <c r="G215" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="I215" s="21" t="s">
+      <c r="I215" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="J215" s="21" t="s">
+      <c r="J215" s="23" t="s">
         <v>203</v>
       </c>
       <c r="K215" s="11" t="s">
@@ -5342,85 +5342,85 @@
       </c>
     </row>
     <row r="216" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B216" s="23"/>
-      <c r="C216" s="20"/>
-      <c r="D216" s="20"/>
+      <c r="B216" s="22"/>
+      <c r="C216" s="24"/>
+      <c r="D216" s="24"/>
       <c r="E216" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G216" s="21"/>
-      <c r="I216" s="21"/>
-      <c r="J216" s="21"/>
+      <c r="G216" s="23"/>
+      <c r="I216" s="23"/>
+      <c r="J216" s="23"/>
     </row>
     <row r="217" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B217" s="23"/>
-      <c r="C217" s="20"/>
-      <c r="D217" s="20"/>
+      <c r="B217" s="22"/>
+      <c r="C217" s="24"/>
+      <c r="D217" s="24"/>
       <c r="E217" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G217" s="21"/>
-      <c r="I217" s="21"/>
-      <c r="J217" s="21"/>
+      <c r="G217" s="23"/>
+      <c r="I217" s="23"/>
+      <c r="J217" s="23"/>
     </row>
     <row r="218" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B218" s="23"/>
-      <c r="C218" s="20"/>
-      <c r="D218" s="20"/>
+      <c r="B218" s="22"/>
+      <c r="C218" s="24"/>
+      <c r="D218" s="24"/>
       <c r="E218" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G218" s="21"/>
-      <c r="I218" s="21"/>
-      <c r="J218" s="21"/>
+      <c r="G218" s="23"/>
+      <c r="I218" s="23"/>
+      <c r="J218" s="23"/>
     </row>
     <row r="219" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B219" s="23"/>
-      <c r="C219" s="20"/>
-      <c r="D219" s="20"/>
+      <c r="B219" s="22"/>
+      <c r="C219" s="24"/>
+      <c r="D219" s="24"/>
       <c r="E219" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G219" s="21"/>
-      <c r="I219" s="21"/>
-      <c r="J219" s="21"/>
+      <c r="G219" s="23"/>
+      <c r="I219" s="23"/>
+      <c r="J219" s="23"/>
     </row>
     <row r="220" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B220" s="23"/>
-      <c r="C220" s="20"/>
-      <c r="D220" s="20"/>
+      <c r="B220" s="22"/>
+      <c r="C220" s="24"/>
+      <c r="D220" s="24"/>
       <c r="E220" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="G220" s="21"/>
-      <c r="I220" s="21"/>
-      <c r="J220" s="21"/>
+      <c r="G220" s="23"/>
+      <c r="I220" s="23"/>
+      <c r="J220" s="23"/>
     </row>
     <row r="221" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B221" s="23"/>
-      <c r="C221" s="20"/>
-      <c r="D221" s="20"/>
+      <c r="B221" s="22"/>
+      <c r="C221" s="24"/>
+      <c r="D221" s="24"/>
       <c r="E221" s="10" t="s">
         <v>38</v>
       </c>
       <c r="F221" s="14"/>
-      <c r="G221" s="21"/>
+      <c r="G221" s="23"/>
       <c r="H221" s="14"/>
-      <c r="I221" s="21"/>
-      <c r="J221" s="21"/>
+      <c r="I221" s="23"/>
+      <c r="J221" s="23"/>
     </row>
     <row r="222" spans="1:11" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B222" s="23"/>
+      <c r="B222" s="22"/>
     </row>
     <row r="223" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="B223" s="23"/>
-      <c r="C223" s="20" t="s">
+      <c r="B223" s="22"/>
+      <c r="C223" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D223" s="20" t="s">
+      <c r="D223" s="24" t="s">
         <v>208</v>
       </c>
       <c r="E223" s="10" t="s">
@@ -5429,13 +5429,13 @@
       <c r="F223" s="10">
         <v>1</v>
       </c>
-      <c r="G223" s="21" t="s">
+      <c r="G223" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="I223" s="21" t="s">
+      <c r="I223" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="J223" s="21" t="s">
+      <c r="J223" s="23" t="s">
         <v>203</v>
       </c>
       <c r="K223" s="10" t="s">
@@ -5443,83 +5443,83 @@
       </c>
     </row>
     <row r="224" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B224" s="23"/>
-      <c r="C224" s="20"/>
-      <c r="D224" s="20"/>
+      <c r="B224" s="22"/>
+      <c r="C224" s="24"/>
+      <c r="D224" s="24"/>
       <c r="E224" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="G224" s="21"/>
-      <c r="I224" s="21"/>
-      <c r="J224" s="21"/>
+      <c r="G224" s="23"/>
+      <c r="I224" s="23"/>
+      <c r="J224" s="23"/>
     </row>
     <row r="225" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B225" s="23"/>
-      <c r="C225" s="20"/>
-      <c r="D225" s="20"/>
+      <c r="B225" s="22"/>
+      <c r="C225" s="24"/>
+      <c r="D225" s="24"/>
       <c r="E225" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G225" s="21"/>
-      <c r="I225" s="21"/>
-      <c r="J225" s="21"/>
+      <c r="G225" s="23"/>
+      <c r="I225" s="23"/>
+      <c r="J225" s="23"/>
     </row>
     <row r="226" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B226" s="23"/>
-      <c r="C226" s="20"/>
-      <c r="D226" s="20"/>
+      <c r="B226" s="22"/>
+      <c r="C226" s="24"/>
+      <c r="D226" s="24"/>
       <c r="E226" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G226" s="21"/>
-      <c r="I226" s="21"/>
-      <c r="J226" s="21"/>
+      <c r="G226" s="23"/>
+      <c r="I226" s="23"/>
+      <c r="J226" s="23"/>
     </row>
     <row r="227" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B227" s="23"/>
-      <c r="C227" s="20"/>
-      <c r="D227" s="20"/>
+      <c r="B227" s="22"/>
+      <c r="C227" s="24"/>
+      <c r="D227" s="24"/>
       <c r="E227" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G227" s="21"/>
-      <c r="I227" s="21"/>
-      <c r="J227" s="21"/>
+      <c r="G227" s="23"/>
+      <c r="I227" s="23"/>
+      <c r="J227" s="23"/>
     </row>
     <row r="228" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B228" s="23"/>
-      <c r="C228" s="20"/>
-      <c r="D228" s="20"/>
+      <c r="B228" s="22"/>
+      <c r="C228" s="24"/>
+      <c r="D228" s="24"/>
       <c r="E228" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="G228" s="21"/>
-      <c r="I228" s="21"/>
-      <c r="J228" s="21"/>
+      <c r="G228" s="23"/>
+      <c r="I228" s="23"/>
+      <c r="J228" s="23"/>
     </row>
     <row r="229" spans="1:11" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B229" s="23"/>
-      <c r="C229" s="20"/>
-      <c r="D229" s="20"/>
+      <c r="B229" s="22"/>
+      <c r="C229" s="24"/>
+      <c r="D229" s="24"/>
       <c r="E229" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G229" s="21"/>
-      <c r="I229" s="21"/>
-      <c r="J229" s="21"/>
+      <c r="G229" s="23"/>
+      <c r="I229" s="23"/>
+      <c r="J229" s="23"/>
     </row>
     <row r="230" spans="1:11" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B230" s="23"/>
+      <c r="B230" s="22"/>
     </row>
     <row r="231" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="B231" s="23"/>
-      <c r="C231" s="20" t="s">
+      <c r="B231" s="22"/>
+      <c r="C231" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D231" s="20" t="s">
+      <c r="D231" s="24" t="s">
         <v>201</v>
       </c>
       <c r="E231" s="10" t="s">
@@ -5528,13 +5528,13 @@
       <c r="F231" s="10">
         <v>1</v>
       </c>
-      <c r="G231" s="21" t="s">
+      <c r="G231" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="I231" s="21" t="s">
+      <c r="I231" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="J231" s="21" t="s">
+      <c r="J231" s="23" t="s">
         <v>203</v>
       </c>
       <c r="K231" s="11" t="s">
@@ -5542,77 +5542,211 @@
       </c>
     </row>
     <row r="232" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B232" s="23"/>
-      <c r="C232" s="20"/>
-      <c r="D232" s="20"/>
+      <c r="B232" s="22"/>
+      <c r="C232" s="24"/>
+      <c r="D232" s="24"/>
       <c r="E232" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G232" s="21"/>
-      <c r="I232" s="21"/>
-      <c r="J232" s="21"/>
+      <c r="G232" s="23"/>
+      <c r="I232" s="23"/>
+      <c r="J232" s="23"/>
     </row>
     <row r="233" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B233" s="23"/>
-      <c r="C233" s="20"/>
-      <c r="D233" s="20"/>
+      <c r="B233" s="22"/>
+      <c r="C233" s="24"/>
+      <c r="D233" s="24"/>
       <c r="E233" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G233" s="21"/>
-      <c r="I233" s="21"/>
-      <c r="J233" s="21"/>
+      <c r="G233" s="23"/>
+      <c r="I233" s="23"/>
+      <c r="J233" s="23"/>
     </row>
     <row r="234" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B234" s="23"/>
-      <c r="C234" s="20"/>
-      <c r="D234" s="20"/>
+      <c r="B234" s="22"/>
+      <c r="C234" s="24"/>
+      <c r="D234" s="24"/>
       <c r="E234" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G234" s="21"/>
-      <c r="I234" s="21"/>
-      <c r="J234" s="21"/>
+      <c r="G234" s="23"/>
+      <c r="I234" s="23"/>
+      <c r="J234" s="23"/>
     </row>
     <row r="235" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B235" s="23"/>
-      <c r="C235" s="20"/>
-      <c r="D235" s="20"/>
+      <c r="B235" s="22"/>
+      <c r="C235" s="24"/>
+      <c r="D235" s="24"/>
       <c r="E235" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G235" s="21"/>
-      <c r="I235" s="21"/>
-      <c r="J235" s="21"/>
+      <c r="G235" s="23"/>
+      <c r="I235" s="23"/>
+      <c r="J235" s="23"/>
     </row>
     <row r="236" spans="1:11" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B236" s="23"/>
-      <c r="C236" s="20"/>
-      <c r="D236" s="20"/>
+      <c r="B236" s="22"/>
+      <c r="C236" s="24"/>
+      <c r="D236" s="24"/>
       <c r="E236" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="G236" s="21"/>
-      <c r="I236" s="21"/>
-      <c r="J236" s="21"/>
+      <c r="G236" s="23"/>
+      <c r="I236" s="23"/>
+      <c r="J236" s="23"/>
     </row>
     <row r="237" spans="1:11" s="14" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B237" s="23"/>
-      <c r="C237" s="20"/>
-      <c r="D237" s="20"/>
+      <c r="B237" s="22"/>
+      <c r="C237" s="24"/>
+      <c r="D237" s="24"/>
       <c r="E237" s="10" t="s">
         <v>38</v>
       </c>
       <c r="F237" s="10"/>
-      <c r="G237" s="21"/>
-      <c r="I237" s="21"/>
-      <c r="J237" s="21"/>
+      <c r="G237" s="23"/>
+      <c r="I237" s="23"/>
+      <c r="J237" s="23"/>
     </row>
     <row r="239" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="240" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="241" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="158">
+    <mergeCell ref="C166:C172"/>
+    <mergeCell ref="D177:D182"/>
+    <mergeCell ref="D184:D189"/>
+    <mergeCell ref="D191:D196"/>
+    <mergeCell ref="D198:D203"/>
+    <mergeCell ref="D205:D210"/>
+    <mergeCell ref="D215:D221"/>
+    <mergeCell ref="D223:D229"/>
+    <mergeCell ref="D231:D237"/>
+    <mergeCell ref="C177:C182"/>
+    <mergeCell ref="C184:C189"/>
+    <mergeCell ref="C191:C196"/>
+    <mergeCell ref="C198:C203"/>
+    <mergeCell ref="C205:C210"/>
+    <mergeCell ref="C215:C221"/>
+    <mergeCell ref="C223:C229"/>
+    <mergeCell ref="C231:C237"/>
+    <mergeCell ref="C98:C103"/>
+    <mergeCell ref="C105:C111"/>
+    <mergeCell ref="C113:C118"/>
+    <mergeCell ref="C120:C125"/>
+    <mergeCell ref="C127:C132"/>
+    <mergeCell ref="C137:C142"/>
+    <mergeCell ref="C144:C149"/>
+    <mergeCell ref="C151:C155"/>
+    <mergeCell ref="C157:C164"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="C31:C37"/>
+    <mergeCell ref="C39:C44"/>
+    <mergeCell ref="C49:C54"/>
+    <mergeCell ref="C63:C68"/>
+    <mergeCell ref="C56:C61"/>
+    <mergeCell ref="C77:C82"/>
+    <mergeCell ref="C84:C93"/>
+    <mergeCell ref="I177:I182"/>
+    <mergeCell ref="J177:J182"/>
+    <mergeCell ref="J184:J189"/>
+    <mergeCell ref="I184:I189"/>
+    <mergeCell ref="L127:L132"/>
+    <mergeCell ref="I205:I210"/>
+    <mergeCell ref="J205:J210"/>
+    <mergeCell ref="I198:I203"/>
+    <mergeCell ref="J198:J203"/>
+    <mergeCell ref="I191:I196"/>
+    <mergeCell ref="J191:J196"/>
+    <mergeCell ref="L151:L155"/>
+    <mergeCell ref="I157:I164"/>
+    <mergeCell ref="J157:J164"/>
+    <mergeCell ref="I166:I172"/>
+    <mergeCell ref="J166:J172"/>
+    <mergeCell ref="L166:L172"/>
+    <mergeCell ref="I137:I142"/>
+    <mergeCell ref="I144:I149"/>
+    <mergeCell ref="J144:J149"/>
+    <mergeCell ref="J151:J155"/>
+    <mergeCell ref="I151:I155"/>
+    <mergeCell ref="K166:K167"/>
+    <mergeCell ref="I231:I237"/>
+    <mergeCell ref="J231:J237"/>
+    <mergeCell ref="G223:G229"/>
+    <mergeCell ref="G215:G221"/>
+    <mergeCell ref="I215:I221"/>
+    <mergeCell ref="J215:J221"/>
+    <mergeCell ref="J223:J229"/>
+    <mergeCell ref="I223:I229"/>
+    <mergeCell ref="G231:G237"/>
+    <mergeCell ref="D166:D172"/>
+    <mergeCell ref="D77:D82"/>
+    <mergeCell ref="D49:D54"/>
+    <mergeCell ref="L105:L111"/>
+    <mergeCell ref="I113:I118"/>
+    <mergeCell ref="J113:J118"/>
+    <mergeCell ref="L113:L118"/>
+    <mergeCell ref="L120:L125"/>
+    <mergeCell ref="I120:I125"/>
+    <mergeCell ref="J120:J125"/>
+    <mergeCell ref="I98:I103"/>
+    <mergeCell ref="J98:J103"/>
+    <mergeCell ref="L98:L103"/>
+    <mergeCell ref="I105:I111"/>
+    <mergeCell ref="J105:J111"/>
+    <mergeCell ref="L10:L15"/>
+    <mergeCell ref="L17:L22"/>
+    <mergeCell ref="L24:L29"/>
+    <mergeCell ref="L39:L44"/>
+    <mergeCell ref="L70:L75"/>
+    <mergeCell ref="L77:L82"/>
+    <mergeCell ref="K77:K78"/>
+    <mergeCell ref="L49:L54"/>
+    <mergeCell ref="K49:K50"/>
+    <mergeCell ref="B3:B44"/>
+    <mergeCell ref="K63:K64"/>
+    <mergeCell ref="K70:K71"/>
+    <mergeCell ref="D63:D68"/>
+    <mergeCell ref="D39:D44"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="I24:I29"/>
+    <mergeCell ref="J24:J29"/>
+    <mergeCell ref="I49:I54"/>
+    <mergeCell ref="J49:J54"/>
+    <mergeCell ref="C70:C75"/>
+    <mergeCell ref="I31:I37"/>
+    <mergeCell ref="J31:J37"/>
+    <mergeCell ref="I39:I45"/>
+    <mergeCell ref="J39:J45"/>
+    <mergeCell ref="I63:I68"/>
+    <mergeCell ref="J63:J68"/>
+    <mergeCell ref="I70:I75"/>
+    <mergeCell ref="J70:J75"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="I127:I132"/>
+    <mergeCell ref="J127:J132"/>
+    <mergeCell ref="J137:J142"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="D17:D22"/>
+    <mergeCell ref="D24:D29"/>
+    <mergeCell ref="D31:D37"/>
+    <mergeCell ref="I3:I8"/>
+    <mergeCell ref="J3:J8"/>
+    <mergeCell ref="I10:I15"/>
+    <mergeCell ref="J10:J15"/>
+    <mergeCell ref="I17:I22"/>
+    <mergeCell ref="J17:J22"/>
+    <mergeCell ref="D70:D75"/>
+    <mergeCell ref="D56:D61"/>
+    <mergeCell ref="I56:I61"/>
+    <mergeCell ref="J56:J61"/>
+    <mergeCell ref="J77:J82"/>
     <mergeCell ref="B77:B93"/>
     <mergeCell ref="B49:B75"/>
     <mergeCell ref="B137:B172"/>
@@ -5637,140 +5771,6 @@
     <mergeCell ref="K98:K99"/>
     <mergeCell ref="I77:I82"/>
     <mergeCell ref="D84:D93"/>
-    <mergeCell ref="I127:I132"/>
-    <mergeCell ref="J127:J132"/>
-    <mergeCell ref="J137:J142"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="D10:D15"/>
-    <mergeCell ref="D17:D22"/>
-    <mergeCell ref="D24:D29"/>
-    <mergeCell ref="D31:D37"/>
-    <mergeCell ref="I3:I8"/>
-    <mergeCell ref="J3:J8"/>
-    <mergeCell ref="I10:I15"/>
-    <mergeCell ref="J10:J15"/>
-    <mergeCell ref="I17:I22"/>
-    <mergeCell ref="J17:J22"/>
-    <mergeCell ref="D70:D75"/>
-    <mergeCell ref="D56:D61"/>
-    <mergeCell ref="I56:I61"/>
-    <mergeCell ref="J56:J61"/>
-    <mergeCell ref="B3:B44"/>
-    <mergeCell ref="K63:K64"/>
-    <mergeCell ref="K70:K71"/>
-    <mergeCell ref="D63:D68"/>
-    <mergeCell ref="D39:D44"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="I24:I29"/>
-    <mergeCell ref="J24:J29"/>
-    <mergeCell ref="I49:I54"/>
-    <mergeCell ref="J49:J54"/>
-    <mergeCell ref="C70:C75"/>
-    <mergeCell ref="L10:L15"/>
-    <mergeCell ref="L17:L22"/>
-    <mergeCell ref="L24:L29"/>
-    <mergeCell ref="L39:L44"/>
-    <mergeCell ref="L70:L75"/>
-    <mergeCell ref="L77:L82"/>
-    <mergeCell ref="K77:K78"/>
-    <mergeCell ref="L49:L54"/>
-    <mergeCell ref="K49:K50"/>
-    <mergeCell ref="I31:I37"/>
-    <mergeCell ref="J31:J37"/>
-    <mergeCell ref="I39:I45"/>
-    <mergeCell ref="J39:J45"/>
-    <mergeCell ref="I63:I68"/>
-    <mergeCell ref="J63:J68"/>
-    <mergeCell ref="I70:I75"/>
-    <mergeCell ref="J70:J75"/>
-    <mergeCell ref="J77:J82"/>
-    <mergeCell ref="D166:D172"/>
-    <mergeCell ref="D77:D82"/>
-    <mergeCell ref="D49:D54"/>
-    <mergeCell ref="L105:L111"/>
-    <mergeCell ref="I113:I118"/>
-    <mergeCell ref="J113:J118"/>
-    <mergeCell ref="L113:L118"/>
-    <mergeCell ref="L120:L125"/>
-    <mergeCell ref="I120:I125"/>
-    <mergeCell ref="J120:J125"/>
-    <mergeCell ref="I98:I103"/>
-    <mergeCell ref="J98:J103"/>
-    <mergeCell ref="L98:L103"/>
-    <mergeCell ref="I105:I111"/>
-    <mergeCell ref="J105:J111"/>
-    <mergeCell ref="I231:I237"/>
-    <mergeCell ref="J231:J237"/>
-    <mergeCell ref="G223:G229"/>
-    <mergeCell ref="G215:G221"/>
-    <mergeCell ref="I215:I221"/>
-    <mergeCell ref="J215:J221"/>
-    <mergeCell ref="J223:J229"/>
-    <mergeCell ref="I223:I229"/>
-    <mergeCell ref="G231:G237"/>
-    <mergeCell ref="I177:I182"/>
-    <mergeCell ref="J177:J182"/>
-    <mergeCell ref="J184:J189"/>
-    <mergeCell ref="I184:I189"/>
-    <mergeCell ref="L127:L132"/>
-    <mergeCell ref="I205:I210"/>
-    <mergeCell ref="J205:J210"/>
-    <mergeCell ref="I198:I203"/>
-    <mergeCell ref="J198:J203"/>
-    <mergeCell ref="I191:I196"/>
-    <mergeCell ref="J191:J196"/>
-    <mergeCell ref="L151:L155"/>
-    <mergeCell ref="I157:I164"/>
-    <mergeCell ref="J157:J164"/>
-    <mergeCell ref="I166:I172"/>
-    <mergeCell ref="J166:J172"/>
-    <mergeCell ref="L166:L172"/>
-    <mergeCell ref="I137:I142"/>
-    <mergeCell ref="I144:I149"/>
-    <mergeCell ref="J144:J149"/>
-    <mergeCell ref="J151:J155"/>
-    <mergeCell ref="I151:I155"/>
-    <mergeCell ref="K166:K167"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="C24:C29"/>
-    <mergeCell ref="C31:C37"/>
-    <mergeCell ref="C39:C44"/>
-    <mergeCell ref="C49:C54"/>
-    <mergeCell ref="C63:C68"/>
-    <mergeCell ref="C56:C61"/>
-    <mergeCell ref="C77:C82"/>
-    <mergeCell ref="C84:C93"/>
-    <mergeCell ref="C98:C103"/>
-    <mergeCell ref="C105:C111"/>
-    <mergeCell ref="C113:C118"/>
-    <mergeCell ref="C120:C125"/>
-    <mergeCell ref="C127:C132"/>
-    <mergeCell ref="C137:C142"/>
-    <mergeCell ref="C144:C149"/>
-    <mergeCell ref="C151:C155"/>
-    <mergeCell ref="C157:C164"/>
-    <mergeCell ref="C166:C172"/>
-    <mergeCell ref="D177:D182"/>
-    <mergeCell ref="D184:D189"/>
-    <mergeCell ref="D191:D196"/>
-    <mergeCell ref="D198:D203"/>
-    <mergeCell ref="D205:D210"/>
-    <mergeCell ref="D215:D221"/>
-    <mergeCell ref="D223:D229"/>
-    <mergeCell ref="D231:D237"/>
-    <mergeCell ref="C177:C182"/>
-    <mergeCell ref="C184:C189"/>
-    <mergeCell ref="C191:C196"/>
-    <mergeCell ref="C198:C203"/>
-    <mergeCell ref="C205:C210"/>
-    <mergeCell ref="C215:C221"/>
-    <mergeCell ref="C223:C229"/>
-    <mergeCell ref="C231:C237"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L39" r:id="rId1" display="https://wordpress.org/support/article/resetting-your-password/" xr:uid="{E2109793-CF5C-4CF2-9ECE-E0EE12594647}"/>
@@ -5782,12 +5782,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5923,15 +5920,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B948061D-A316-4845-8B7E-2AC163B12D67}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C69DD728-9915-4AE5-BD17-53118132EF17}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5955,10 +5956,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C69DD728-9915-4AE5-BD17-53118132EF17}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B948061D-A316-4845-8B7E-2AC163B12D67}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>